<commit_message>
Working on Hardware Manual
</commit_message>
<xml_diff>
--- a/hard/CPU/v0/board/bom/BOM_PLsi_0.xlsx
+++ b/hard/CPU/v0/board/bom/BOM_PLsi_0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="v0 - Digital " sheetId="1" state="visible" r:id="rId2"/>
@@ -21,12 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="85">
   <si>
     <t xml:space="preserve">Item</t>
   </si>
   <si>
-    <t xml:space="preserve">Designator</t>
+    <t xml:space="preserve">Component TAG</t>
   </si>
   <si>
     <t xml:space="preserve">Description</t>
@@ -86,7 +86,7 @@
     <t xml:space="preserve">Touch Screen Display SD Card connection</t>
   </si>
   <si>
-    <t xml:space="preserve">U1 and U2 - Optional socket</t>
+    <t xml:space="preserve">U1 and U2 – Socket</t>
   </si>
   <si>
     <t xml:space="preserve">Dupont 2.54mm Female strip</t>
@@ -96,198 +96,254 @@
   </si>
   <si>
     <t xml:space="preserve">Female sockets for ESP32 and Display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dupont 3 pins male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 pins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optional – External 5V use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDR-IDC-2.54-2X4P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optional - I2C expansion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacitor 1000uF 9V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPTO1, OPTO2, OPTO3, OPTO4, OPTO5, OPTO6, OPTO7, OPTO8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optocupler PC817</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optocouplers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z1, Z2, Z3, Z4, Z5, Z6, Z7, Z8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diode 5v1 – Zenner 1w</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digital Inputs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I0, I1, I2, I3, I4, I5, I6, I7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leds 3mm Color 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leds digital inputs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q0, Q1, Q2, Q3, Q4, Q5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leds 3mm Color 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leds digital outputs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3, R6, R9, R12, R13, R16, R19, R24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor 10k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistors digital inputs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1, R5, R8, R11, R14, R17, R20, R23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor 1K x 1/2W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2, R4, R7, R10, R15, R18, R21, R22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor 510 ohms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R31, R32, R33, R34, R35, R36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor 330 ohms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digital outputs leds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELAY1, RELAY2, RELAY3, RELAY4, RELAY5, RELAY6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SRD-05VDC-SL-C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output Relays</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPTO1, OPTO2, OPTO3, OPTO4, OPTO5, OPTO6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z1, Z2, Z3, Z4, Z5, Z6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I0, I1, I2, I3, I4, I5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q0, Q1, Q2, Q3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R3, R6, R9, R12, R19, R24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1, R5, R8, R11, R20, R23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R2, R4, R7, R10, R21, R22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R31, R32, R33, R34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RELAY1, RELAY2, RELAY3, RELAY4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D1, D2, D3, D4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diode 1N4148</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analog Inputs protection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R25, R26, R37, R38, R39, R40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor 10k  1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analog Inputs ⅓ divisor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R27,R29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor 5k1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analog outputs gain divisor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R28,R30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor 3k3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TLV2462CP</t>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="8"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Analog outputs </t>
+      <t xml:space="preserve">5V</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Optional)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Dupont 3 pins male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 pins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional – External 5V use</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Rail to Rail Op Amplifier </t>
+      <t xml:space="preserve">P4</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Optional)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">HDR-IDC-2.54-2X4P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional - I2C expansion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor 1000uF 9V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTO1, OPTO2, OPTO3, OPTO4, OPTO5, OPTO6, OPTO7, OPTO8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optocupler PC817</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optocouplers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z1, Z2, Z3, Z4, Z5, Z6, Z7, Z8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diode 5v1 – Zenner 1w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital Inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I0, I1, I2, I3, I4, I5, I6, I7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leds 3mm Color 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leds digital inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q0, Q1, Q2, Q3, Q4, Q5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leds 3mm Color 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leds digital outputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3, R6, R9, R12, R13, R16, R19, R24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor 10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistors digital inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1, R5, R8, R11, R14, R17, R20, R23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor 1K x 1/2W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2, R4, R7, R10, R15, R18, R21, R22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor 510 ohms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R31, R32, R33, R34, R35, R36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor 330 ohms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital outputs leds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RELAY1, RELAY2, RELAY3, RELAY4, RELAY5, RELAY6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRD-05VDC-SL-C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output Relays</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">5V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Optional)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">P4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Optional)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTO1, OPTO2, OPTO3, OPTO4, OPTO5, OPTO6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z1, Z2, Z3, Z4, Z5, Z6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I0, I1, I2, I3, I4, I5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q0, Q1, Q2, Q3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3, R6, R9, R12, R19, R24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1, R5, R8, R11, R20, R23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2, R4, R7, R10, R21, R22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R31, R32, R33, R34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RELAY1, RELAY2, RELAY3, RELAY4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1, D2, D3, D4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diode 1N4148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog Inputs protection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R25, R26, R37, R38, R39, R40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor 10k  1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog Inputs ⅓ divisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R27,R29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor 5k1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog outputs gain divisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R28,R30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor 3k3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLV2462CP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog outputs Rail to Rail Op Amplifier </t>
   </si>
 </sst>
 </file>
@@ -297,7 +353,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -328,10 +384,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -414,7 +476,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -438,11 +500,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -519,24 +581,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="34.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="34.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="36.88"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="6" style="4" width="8.69"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="6" style="4" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="4" width="11.52"/>
   </cols>
   <sheetData>
@@ -869,8 +931,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -879,24 +941,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="9.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="30.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="30.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="26.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="46.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="6" style="2" width="8.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="10" width="46.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="6" style="2" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1022" style="2" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -922,7 +984,7 @@
       <c r="A2" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="12" t="s">
@@ -931,7 +993,7 @@
       <c r="D2" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -939,7 +1001,7 @@
       <c r="A3" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="12" t="s">
@@ -948,7 +1010,7 @@
       <c r="D3" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="13" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="11"/>
@@ -957,7 +1019,7 @@
       <c r="A4" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="12" t="s">
@@ -966,7 +1028,7 @@
       <c r="D4" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="13" t="s">
         <v>13</v>
       </c>
     </row>
@@ -974,7 +1036,7 @@
       <c r="A5" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="12" t="s">
@@ -983,7 +1045,7 @@
       <c r="D5" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -991,7 +1053,7 @@
       <c r="A6" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="12" t="s">
@@ -1000,7 +1062,7 @@
       <c r="D6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="13" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1008,7 +1070,7 @@
       <c r="A7" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="13" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="12" t="s">
@@ -1017,7 +1079,7 @@
       <c r="D7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="13" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1025,8 +1087,8 @@
       <c r="A8" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>25</v>
+      <c r="B8" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>26</v>
@@ -1034,7 +1096,7 @@
       <c r="D8" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="13" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1042,8 +1104,8 @@
       <c r="A9" s="12" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>29</v>
+      <c r="B9" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>30</v>
@@ -1051,7 +1113,7 @@
       <c r="D9" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="13" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1059,7 +1121,7 @@
       <c r="A10" s="12" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="13" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -1068,16 +1130,16 @@
       <c r="D10" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>60</v>
+      <c r="B11" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>36</v>
@@ -1085,7 +1147,7 @@
       <c r="D11" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="13" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1093,8 +1155,8 @@
       <c r="A12" s="12" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>61</v>
+      <c r="B12" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>39</v>
@@ -1102,7 +1164,7 @@
       <c r="D12" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="13" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1110,8 +1172,8 @@
       <c r="A13" s="12" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>62</v>
+      <c r="B13" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>42</v>
@@ -1119,7 +1181,7 @@
       <c r="D13" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1127,8 +1189,8 @@
       <c r="A14" s="12" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>63</v>
+      <c r="B14" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>45</v>
@@ -1136,7 +1198,7 @@
       <c r="D14" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="13" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1144,8 +1206,8 @@
       <c r="A15" s="12" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>64</v>
+      <c r="B15" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>48</v>
@@ -1153,7 +1215,7 @@
       <c r="D15" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1161,8 +1223,8 @@
       <c r="A16" s="12" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>65</v>
+      <c r="B16" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>51</v>
@@ -1170,7 +1232,7 @@
       <c r="D16" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1178,8 +1240,8 @@
       <c r="A17" s="12" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>66</v>
+      <c r="B17" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>53</v>
@@ -1187,7 +1249,7 @@
       <c r="D17" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="13" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1195,8 +1257,8 @@
       <c r="A18" s="12" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>67</v>
+      <c r="B18" s="13" t="s">
+        <v>69</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>55</v>
@@ -1204,16 +1266,16 @@
       <c r="D18" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>68</v>
+      <c r="B19" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>58</v>
@@ -1221,7 +1283,7 @@
       <c r="D19" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="13" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1229,85 +1291,85 @@
       <c r="A20" s="12" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>69</v>
+      <c r="B20" s="13" t="s">
+        <v>71</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D20" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>71</v>
+      <c r="E20" s="13" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>72</v>
+      <c r="B21" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D21" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>74</v>
+      <c r="E21" s="13" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>75</v>
+      <c r="B22" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D22" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>77</v>
+      <c r="E22" s="13" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>78</v>
+      <c r="B23" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D23" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>77</v>
+      <c r="E23" s="13" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>80</v>
+      <c r="B24" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D24" s="12" t="n">
         <v>1</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1316,10 +1378,11 @@
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="10"/>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>